<commit_message>
fix a bug in GenerateReport_Test
</commit_message>
<xml_diff>
--- a/AutoRegularInspectionTestProject/外观检查.xlsx
+++ b/AutoRegularInspectionTestProject/外观检查.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924BDD1A-DBF0-453D-B1AD-6CD25FF8B5BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFEBC70-A3FB-43D8-A338-169DB672DE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="3765" windowWidth="28125" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
   <si>
     <t>序号</t>
   </si>
@@ -148,6 +148,14 @@
   </si>
   <si>
     <t>构件类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -190,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -200,6 +208,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -490,7 +501,7 @@
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +523,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -558,8 +572,11 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -580,7 +597,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -602,8 +619,11 @@
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -626,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -634,7 +654,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -642,7 +662,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -650,7 +670,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -658,7 +678,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -666,7 +686,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -674,7 +694,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -682,7 +702,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -690,7 +710,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -698,7 +718,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -829,17 +849,15 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -849,7 +867,7 @@
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -871,8 +889,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -895,7 +916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -917,8 +938,9 @@
       <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -926,7 +948,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -934,7 +956,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -942,7 +964,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -950,7 +972,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -958,7 +980,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -974,11 +996,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -988,7 +1008,7 @@
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,8 +1030,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1034,7 +1057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1056,8 +1079,9 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1079,8 +1103,11 @@
       <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1103,7 +1130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1126,7 +1153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>